<commit_message>
Signed-off-by: mahmouddgamall <mahmouddgamall93@gmail.com> in this commit, a new question has been added, as well as the updated CYRS with very minor changes
</commit_message>
<xml_diff>
--- a/Input Documents/SIQ Q&A.xlsx
+++ b/Input Documents/SIQ Q&A.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D090C9-263C-4E40-BD76-45BF8522DA9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Questions</t>
   </si>
@@ -50,12 +51,15 @@
 All switches are connected as an input for the controller
 </t>
   </si>
+  <si>
+    <t>How much do you need the delay in the animations to be?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +95,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -118,7 +128,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -132,6 +142,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -155,7 +168,7 @@
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -173,7 +186,7 @@
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -191,7 +204,7 @@
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -209,7 +222,7 @@
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -225,11 +238,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B4" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" headerRowCellStyle="Neutral">
-  <autoFilter ref="A1:B4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B5" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" headerRowCellStyle="Neutral">
+  <autoFilter ref="A1:B5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Questions" dataDxfId="1"/>
-    <tableColumn id="2" name="Answers" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Questions" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Answers" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -490,27 +503,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="88.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21">
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -518,7 +531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="31.5">
+    <row r="2" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -526,7 +539,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="63">
+    <row r="3" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -534,7 +547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="110.25">
+    <row r="4" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -542,19 +555,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:2" ht="15.75">
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:2" ht="15.75">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:2" ht="15.75">
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
     </row>

</xml_diff>